<commit_message>
Aggiornamento bandi Nitti e Rainoldi
Aggiornamento bandi Nitti e Rainoldi
</commit_message>
<xml_diff>
--- a/Bandi/AdolescentiARischio/anagraficaadolescenti.xlsx
+++ b/Bandi/AdolescentiARischio/anagraficaadolescenti.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26122"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="560" yWindow="560" windowWidth="25040" windowHeight="14900" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="560" yWindow="560" windowWidth="25040" windowHeight="14900" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="profili" sheetId="1" r:id="rId1"/>
@@ -367,8 +367,60 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="147">
+  <cellStyleXfs count="199">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -522,7 +574,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="147">
+  <cellStyles count="199">
     <cellStyle name="Collegamento ipertestuale" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Collegamento ipertestuale" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Collegamento ipertestuale" xfId="5" builtinId="8" hidden="1"/>
@@ -596,6 +648,32 @@
     <cellStyle name="Collegamento ipertestuale" xfId="141" builtinId="8" hidden="1"/>
     <cellStyle name="Collegamento ipertestuale" xfId="143" builtinId="8" hidden="1"/>
     <cellStyle name="Collegamento ipertestuale" xfId="145" builtinId="8" hidden="1"/>
+    <cellStyle name="Collegamento ipertestuale" xfId="147" builtinId="8" hidden="1"/>
+    <cellStyle name="Collegamento ipertestuale" xfId="149" builtinId="8" hidden="1"/>
+    <cellStyle name="Collegamento ipertestuale" xfId="151" builtinId="8" hidden="1"/>
+    <cellStyle name="Collegamento ipertestuale" xfId="153" builtinId="8" hidden="1"/>
+    <cellStyle name="Collegamento ipertestuale" xfId="155" builtinId="8" hidden="1"/>
+    <cellStyle name="Collegamento ipertestuale" xfId="157" builtinId="8" hidden="1"/>
+    <cellStyle name="Collegamento ipertestuale" xfId="159" builtinId="8" hidden="1"/>
+    <cellStyle name="Collegamento ipertestuale" xfId="161" builtinId="8" hidden="1"/>
+    <cellStyle name="Collegamento ipertestuale" xfId="163" builtinId="8" hidden="1"/>
+    <cellStyle name="Collegamento ipertestuale" xfId="165" builtinId="8" hidden="1"/>
+    <cellStyle name="Collegamento ipertestuale" xfId="167" builtinId="8" hidden="1"/>
+    <cellStyle name="Collegamento ipertestuale" xfId="169" builtinId="8" hidden="1"/>
+    <cellStyle name="Collegamento ipertestuale" xfId="171" builtinId="8" hidden="1"/>
+    <cellStyle name="Collegamento ipertestuale" xfId="173" builtinId="8" hidden="1"/>
+    <cellStyle name="Collegamento ipertestuale" xfId="175" builtinId="8" hidden="1"/>
+    <cellStyle name="Collegamento ipertestuale" xfId="177" builtinId="8" hidden="1"/>
+    <cellStyle name="Collegamento ipertestuale" xfId="179" builtinId="8" hidden="1"/>
+    <cellStyle name="Collegamento ipertestuale" xfId="181" builtinId="8" hidden="1"/>
+    <cellStyle name="Collegamento ipertestuale" xfId="183" builtinId="8" hidden="1"/>
+    <cellStyle name="Collegamento ipertestuale" xfId="185" builtinId="8" hidden="1"/>
+    <cellStyle name="Collegamento ipertestuale" xfId="187" builtinId="8" hidden="1"/>
+    <cellStyle name="Collegamento ipertestuale" xfId="189" builtinId="8" hidden="1"/>
+    <cellStyle name="Collegamento ipertestuale" xfId="191" builtinId="8" hidden="1"/>
+    <cellStyle name="Collegamento ipertestuale" xfId="193" builtinId="8" hidden="1"/>
+    <cellStyle name="Collegamento ipertestuale" xfId="195" builtinId="8" hidden="1"/>
+    <cellStyle name="Collegamento ipertestuale" xfId="197" builtinId="8" hidden="1"/>
     <cellStyle name="Collegamento visitato" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Collegamento visitato" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Collegamento visitato" xfId="6" builtinId="9" hidden="1"/>
@@ -669,6 +747,32 @@
     <cellStyle name="Collegamento visitato" xfId="142" builtinId="9" hidden="1"/>
     <cellStyle name="Collegamento visitato" xfId="144" builtinId="9" hidden="1"/>
     <cellStyle name="Collegamento visitato" xfId="146" builtinId="9" hidden="1"/>
+    <cellStyle name="Collegamento visitato" xfId="148" builtinId="9" hidden="1"/>
+    <cellStyle name="Collegamento visitato" xfId="150" builtinId="9" hidden="1"/>
+    <cellStyle name="Collegamento visitato" xfId="152" builtinId="9" hidden="1"/>
+    <cellStyle name="Collegamento visitato" xfId="154" builtinId="9" hidden="1"/>
+    <cellStyle name="Collegamento visitato" xfId="156" builtinId="9" hidden="1"/>
+    <cellStyle name="Collegamento visitato" xfId="158" builtinId="9" hidden="1"/>
+    <cellStyle name="Collegamento visitato" xfId="160" builtinId="9" hidden="1"/>
+    <cellStyle name="Collegamento visitato" xfId="162" builtinId="9" hidden="1"/>
+    <cellStyle name="Collegamento visitato" xfId="164" builtinId="9" hidden="1"/>
+    <cellStyle name="Collegamento visitato" xfId="166" builtinId="9" hidden="1"/>
+    <cellStyle name="Collegamento visitato" xfId="168" builtinId="9" hidden="1"/>
+    <cellStyle name="Collegamento visitato" xfId="170" builtinId="9" hidden="1"/>
+    <cellStyle name="Collegamento visitato" xfId="172" builtinId="9" hidden="1"/>
+    <cellStyle name="Collegamento visitato" xfId="174" builtinId="9" hidden="1"/>
+    <cellStyle name="Collegamento visitato" xfId="176" builtinId="9" hidden="1"/>
+    <cellStyle name="Collegamento visitato" xfId="178" builtinId="9" hidden="1"/>
+    <cellStyle name="Collegamento visitato" xfId="180" builtinId="9" hidden="1"/>
+    <cellStyle name="Collegamento visitato" xfId="182" builtinId="9" hidden="1"/>
+    <cellStyle name="Collegamento visitato" xfId="184" builtinId="9" hidden="1"/>
+    <cellStyle name="Collegamento visitato" xfId="186" builtinId="9" hidden="1"/>
+    <cellStyle name="Collegamento visitato" xfId="188" builtinId="9" hidden="1"/>
+    <cellStyle name="Collegamento visitato" xfId="190" builtinId="9" hidden="1"/>
+    <cellStyle name="Collegamento visitato" xfId="192" builtinId="9" hidden="1"/>
+    <cellStyle name="Collegamento visitato" xfId="194" builtinId="9" hidden="1"/>
+    <cellStyle name="Collegamento visitato" xfId="196" builtinId="9" hidden="1"/>
+    <cellStyle name="Collegamento visitato" xfId="198" builtinId="9" hidden="1"/>
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1000,8 +1104,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1202,7 +1306,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>

</xml_diff>